<commit_message>
added card number to card
</commit_message>
<xml_diff>
--- a/mass_producer/技能.xlsx
+++ b/mass_producer/技能.xlsx
@@ -5,10 +5,10 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/yifeichen/WorkSpace/GithubRepos/Wizard-s-Deck/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/yifeichen/WorkSpace/GithubRepos/Wizard-s-Deck/mass_producer/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{7136697A-285B-B245-B5F2-397E26356D0E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{194F8179-8ED7-5A43-A298-5F2E96A733F9}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="680" yWindow="740" windowWidth="28040" windowHeight="17260" xr2:uid="{A1D7679E-E48B-4C4E-B565-963420B95A63}"/>
   </bookViews>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="16" uniqueCount="16">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="17" uniqueCount="16">
   <si>
     <t>编号</t>
   </si>
@@ -77,13 +77,13 @@
     <t>法术·AOE</t>
   </si>
   <si>
-    <t>4风</t>
-  </si>
-  <si>
     <t>哈哈哈哈哈</t>
   </si>
   <si>
     <t>哈哈哈哈哈哈</t>
+  </si>
+  <si>
+    <t>4风1火1水1暗1光</t>
   </si>
 </sst>
 </file>
@@ -446,7 +446,7 @@
   <dimension ref="A1:K2"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="J2" sqref="J2"/>
+      <selection activeCell="E2" sqref="E2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -498,16 +498,19 @@
         <v>12</v>
       </c>
       <c r="E2" t="s">
-        <v>13</v>
+        <v>15</v>
       </c>
       <c r="F2">
         <v>5</v>
       </c>
+      <c r="H2" t="s">
+        <v>15</v>
+      </c>
       <c r="I2" t="s">
+        <v>13</v>
+      </c>
+      <c r="J2" t="s">
         <v>14</v>
-      </c>
-      <c r="J2" t="s">
-        <v>15</v>
       </c>
     </row>
   </sheetData>

</xml_diff>